<commit_message>
updated files for marci's paper
</commit_message>
<xml_diff>
--- a/working/SmeltzPFAS/SmeltzPFAS-Clint-Level4.xlsx
+++ b/working/SmeltzPFAS/SmeltzPFAS-Clint-Level4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitroTKstats\working\SmeltzPFAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\SmeltzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{653C8082-F20D-4C46-8C64-FA676A47CE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{542A41C2-74A6-495F-BE29-C8D903FF5830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="27375" windowHeight="13740"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="SmeltzPFAS-Clint-Level4" sheetId="1" r:id="rId1"/>
@@ -584,9 +584,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -662,7 +661,7 @@
     <tableColumn id="11" name="Sat.pValue"/>
     <tableColumn id="12" name="degrades.pValue"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -969,23 +968,23 @@
       <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1034,13 +1033,13 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>10.5</v>
+        <v>10.7</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>13.9</v>
+        <v>14.2</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -1052,7 +1051,7 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>2.7900000000000001E-2</v>
+        <v>3.2800000000000003E-2</v>
       </c>
       <c r="K2">
         <v>0.75</v>
@@ -1061,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1072,13 +1071,13 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>9.9700000000000006</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>7.37</v>
+        <v>7.6</v>
       </c>
       <c r="F3">
-        <v>12.3</v>
+        <v>12.1</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -1089,17 +1088,17 @@
       <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1">
-        <v>2.0000000000000002E-5</v>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.75</v>
+        <v>0.748</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1131,13 +1130,13 @@
         <v>0.999</v>
       </c>
       <c r="K4">
-        <v>0.75</v>
+        <v>0.749</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1166,16 +1165,16 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.998</v>
+        <v>0.999</v>
       </c>
       <c r="K5">
-        <v>0.75</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1207,13 +1206,13 @@
         <v>0.98599999999999999</v>
       </c>
       <c r="K6">
-        <v>0.753</v>
+        <v>0.748</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1245,13 +1244,13 @@
         <v>0.999</v>
       </c>
       <c r="K7">
-        <v>0.751</v>
+        <v>0.749</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>0.999</v>
       </c>
       <c r="K8">
-        <v>0.752</v>
+        <v>0.747</v>
       </c>
       <c r="L8">
         <v>1</v>

</xml_diff>